<commit_message>
feat(api): update new xlsx template
</commit_message>
<xml_diff>
--- a/apps/api/templates/xlsx-template.xlsx
+++ b/apps/api/templates/xlsx-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6CE4E096-72BC-4691-8155-FA6418EF1010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{30F7BD5F-E734-44FE-A436-9508585AD847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,24 +39,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="129">
-  <si>
-    <t>TRƯỜNG CAO ĐẲNG HẬU CẦN 2</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="128">
+  <si>
+    <t>${upperUnitName}</t>
   </si>
   <si>
     <t>CỘNG HÒA XÃ HỘI CHỦ NGHĨA VIỆT NAM</t>
   </si>
   <si>
-    <t>TIỂU ĐOÀN 2</t>
+    <t>${unitName}</t>
   </si>
   <si>
     <t>Độc lập – Tự do - Hạnh phúc</t>
   </si>
   <si>
     <t>Thành phố Hồ Chí Minh, ngày ${day} tháng ${month} năm ${year}</t>
-  </si>
-  <si>
-    <t>MẬT</t>
   </si>
   <si>
     <t>THỐNG KÊ</t>
@@ -264,85 +261,85 @@
     <t>Tổng</t>
   </si>
   <si>
-    <t>=SUM(C10:C${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(D10:D${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(E10:E${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(F10:F${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(G10:G${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(H10:H${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(I10:I${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(J10:J${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(K10:K${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(L10:L${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(M10:M${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(N10:N${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(O10:O${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(P10:P${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(Q10:Q${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(R10:R${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(S10:S${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(T10:T${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(U10:U${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(V10:V${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(W10:W${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(X10:X${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(Y10:Y${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(Z10:Z${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(AA10:AA${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(AB10:AB${endRowNum})</t>
-  </si>
-  <si>
-    <t>=SUM(AC10:AC${endRowNum})</t>
+    <t>${total.total}</t>
+  </si>
+  <si>
+    <t>${total.totalColonel}</t>
+  </si>
+  <si>
+    <t>${total.totalLieutenant}</t>
+  </si>
+  <si>
+    <t>${total.totalProSoldierCommander}</t>
+  </si>
+  <si>
+    <t>${total.totalProSoldier}</t>
+  </si>
+  <si>
+    <t>${total.totalSoldier}</t>
+  </si>
+  <si>
+    <t>${total.totalWorker}</t>
+  </si>
+  <si>
+    <t>${total.kinh}</t>
+  </si>
+  <si>
+    <t>${total.hoa}</t>
+  </si>
+  <si>
+    <t>${total.otherEthnics}</t>
+  </si>
+  <si>
+    <t>${total.buddhism}</t>
+  </si>
+  <si>
+    <t>${total.christianity}</t>
+  </si>
+  <si>
+    <t>${total.caodaism}</t>
+  </si>
+  <si>
+    <t>${total.protestantism}</t>
+  </si>
+  <si>
+    <t>${total.hoahaoism}</t>
+  </si>
+  <si>
+    <t>${total.secondarySchool}</t>
+  </si>
+  <si>
+    <t>${total.highSchool}</t>
+  </si>
+  <si>
+    <t>${total.universityAndOthers}</t>
+  </si>
+  <si>
+    <t>${total.postGraduate}</t>
+  </si>
+  <si>
+    <t>${total.cpv}</t>
+  </si>
+  <si>
+    <t>${total.hcyu}</t>
+  </si>
+  <si>
+    <t>${total.cm}</t>
+  </si>
+  <si>
+    <t>${total.nguy}</t>
+  </si>
+  <si>
+    <t>${total.aboard}</t>
+  </si>
+  <si>
+    <t>${total.male}</t>
+  </si>
+  <si>
+    <t>${total.female}</t>
+  </si>
+  <si>
+    <t>${total.note}</t>
   </si>
   <si>
     <t>TT</t>
@@ -434,7 +431,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -537,6 +534,12 @@
     <font>
       <b/>
       <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -666,7 +669,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -735,91 +738,61 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -833,44 +806,80 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2738,128 +2747,127 @@
   <dimension ref="A1:BE34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="15"/>
   <cols>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:57" ht="16.5">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
       <c r="I1" s="18"/>
-      <c r="J1" s="39" t="s">
+      <c r="J1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
-      <c r="X1" s="39"/>
-      <c r="Y1" s="39"/>
-      <c r="Z1" s="39"/>
-      <c r="AA1" s="39"/>
-      <c r="AB1" s="39"/>
-      <c r="AC1" s="39"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="61"/>
+      <c r="V1" s="61"/>
+      <c r="W1" s="61"/>
+      <c r="X1" s="61"/>
+      <c r="Y1" s="61"/>
+      <c r="Z1" s="61"/>
+      <c r="AA1" s="61"/>
+      <c r="AB1" s="61"/>
+      <c r="AC1" s="61"/>
       <c r="AD1" s="8"/>
     </row>
     <row r="2" spans="1:57" ht="16.5">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
       <c r="I2" s="17"/>
-      <c r="J2" s="41" t="s">
+      <c r="J2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="41"/>
-      <c r="T2" s="41"/>
-      <c r="U2" s="41"/>
-      <c r="V2" s="41"/>
-      <c r="W2" s="41"/>
-      <c r="X2" s="41"/>
-      <c r="Y2" s="41"/>
-      <c r="Z2" s="41"/>
-      <c r="AA2" s="41"/>
-      <c r="AB2" s="41"/>
-      <c r="AC2" s="41"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="63"/>
+      <c r="W2" s="63"/>
+      <c r="X2" s="63"/>
+      <c r="Y2" s="63"/>
+      <c r="Z2" s="63"/>
+      <c r="AA2" s="63"/>
+      <c r="AB2" s="63"/>
+      <c r="AC2" s="63"/>
       <c r="AD2" s="8"/>
     </row>
     <row r="3" spans="1:57" ht="16.5">
-      <c r="A3" s="29"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
       <c r="D3" s="15"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
-      <c r="J3" s="42" t="s">
+      <c r="J3" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="42"/>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="42"/>
-      <c r="S3" s="42"/>
-      <c r="T3" s="42"/>
-      <c r="U3" s="42"/>
-      <c r="V3" s="42"/>
-      <c r="W3" s="42"/>
-      <c r="X3" s="42"/>
-      <c r="Y3" s="42"/>
-      <c r="Z3" s="42"/>
-      <c r="AA3" s="42"/>
-      <c r="AB3" s="42"/>
-      <c r="AC3" s="42"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="64"/>
+      <c r="T3" s="64"/>
+      <c r="U3" s="64"/>
+      <c r="V3" s="64"/>
+      <c r="W3" s="64"/>
+      <c r="X3" s="64"/>
+      <c r="Y3" s="64"/>
+      <c r="Z3" s="64"/>
+      <c r="AA3" s="64"/>
+      <c r="AB3" s="64"/>
+      <c r="AC3" s="64"/>
       <c r="AD3" s="8"/>
     </row>
     <row r="4" spans="1:57" ht="16.5">
-      <c r="A4" s="28"/>
-      <c r="B4" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
@@ -2888,68 +2896,68 @@
       <c r="AD4" s="8"/>
     </row>
     <row r="5" spans="1:57" ht="18.75">
-      <c r="A5" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
-      <c r="N5" s="44"/>
-      <c r="O5" s="44"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="44"/>
-      <c r="S5" s="44"/>
-      <c r="T5" s="44"/>
-      <c r="U5" s="44"/>
-      <c r="V5" s="44"/>
-      <c r="W5" s="44"/>
-      <c r="X5" s="44"/>
-      <c r="Y5" s="44"/>
-      <c r="Z5" s="44"/>
+      <c r="A5" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="65"/>
+      <c r="P5" s="65"/>
+      <c r="Q5" s="65"/>
+      <c r="R5" s="65"/>
+      <c r="S5" s="65"/>
+      <c r="T5" s="65"/>
+      <c r="U5" s="65"/>
+      <c r="V5" s="65"/>
+      <c r="W5" s="65"/>
+      <c r="X5" s="65"/>
+      <c r="Y5" s="65"/>
+      <c r="Z5" s="65"/>
       <c r="AA5" s="8"/>
       <c r="AB5" s="8"/>
       <c r="AC5" s="8"/>
       <c r="AD5" s="8"/>
     </row>
     <row r="6" spans="1:57" ht="19.5">
-      <c r="A6" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="45"/>
-      <c r="S6" s="45"/>
-      <c r="T6" s="45"/>
-      <c r="U6" s="45"/>
-      <c r="V6" s="45"/>
-      <c r="W6" s="45"/>
-      <c r="X6" s="45"/>
-      <c r="Y6" s="45"/>
-      <c r="Z6" s="45"/>
+      <c r="A6" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="66"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="66"/>
+      <c r="P6" s="66"/>
+      <c r="Q6" s="66"/>
+      <c r="R6" s="66"/>
+      <c r="S6" s="66"/>
+      <c r="T6" s="66"/>
+      <c r="U6" s="66"/>
+      <c r="V6" s="66"/>
+      <c r="W6" s="66"/>
+      <c r="X6" s="66"/>
+      <c r="Y6" s="66"/>
+      <c r="Z6" s="66"/>
       <c r="AA6" s="14"/>
       <c r="AB6" s="8"/>
       <c r="AC6" s="8"/>
@@ -2988,320 +2996,322 @@
       <c r="AD7" s="8"/>
     </row>
     <row r="8" spans="1:57">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="67" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="C8" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="D8" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="49" t="s">
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="49" t="s">
+      <c r="L8" s="71"/>
+      <c r="M8" s="72"/>
+      <c r="N8" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="L8" s="50"/>
-      <c r="M8" s="51"/>
-      <c r="N8" s="49" t="s">
+      <c r="O8" s="71"/>
+      <c r="P8" s="71"/>
+      <c r="Q8" s="71"/>
+      <c r="R8" s="72"/>
+      <c r="S8" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="O8" s="50"/>
-      <c r="P8" s="50"/>
-      <c r="Q8" s="50"/>
-      <c r="R8" s="51"/>
-      <c r="S8" s="49" t="s">
+      <c r="T8" s="71"/>
+      <c r="U8" s="71"/>
+      <c r="V8" s="72"/>
+      <c r="W8" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="T8" s="50"/>
-      <c r="U8" s="50"/>
-      <c r="V8" s="51"/>
-      <c r="W8" s="46" t="s">
+      <c r="X8" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="X8" s="46" t="s">
+      <c r="Y8" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="Y8" s="52" t="s">
+      <c r="Z8" s="50"/>
+      <c r="AA8" s="51"/>
+      <c r="AB8" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="Z8" s="53"/>
-      <c r="AA8" s="54"/>
-      <c r="AB8" s="32" t="s">
+      <c r="AC8" s="55"/>
+      <c r="AD8" s="56" t="s">
         <v>18</v>
-      </c>
-      <c r="AC8" s="33"/>
-      <c r="AD8" s="34" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:57" ht="82.5">
-      <c r="A9" s="47"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="47"/>
+      <c r="A9" s="68"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="68"/>
       <c r="D9" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="F9" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="G9" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="H9" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="I9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="J9" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="30" t="s">
+      <c r="K9" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="K9" s="30" t="s">
+      <c r="L9" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="L9" s="30" t="s">
+      <c r="M9" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="N9" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="N9" s="30" t="s">
+      <c r="O9" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="O9" s="30" t="s">
+      <c r="P9" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="P9" s="30" t="s">
+      <c r="Q9" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="Q9" s="30" t="s">
+      <c r="R9" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="R9" s="12" t="s">
+      <c r="S9" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="S9" s="30" t="s">
+      <c r="T9" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="T9" s="30" t="s">
+      <c r="U9" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="U9" s="30" t="s">
+      <c r="V9" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="V9" s="10" t="s">
+      <c r="W9" s="68"/>
+      <c r="X9" s="68"/>
+      <c r="Y9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="W9" s="47"/>
-      <c r="X9" s="47"/>
-      <c r="Y9" s="10" t="s">
+      <c r="Z9" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="Z9" s="11" t="s">
+      <c r="AA9" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="AA9" s="10" t="s">
+      <c r="AB9" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="AB9" s="19" t="s">
+      <c r="AC9" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="AC9" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD9" s="35"/>
+      <c r="AD9" s="57"/>
     </row>
     <row r="10" spans="1:57" ht="52.5">
       <c r="A10" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="C10" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="D10" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="E10" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="F10" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="G10" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="H10" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="I10" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="J10" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="I10" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="J10" s="22" t="s">
+      <c r="K10" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="K10" s="21" t="s">
+      <c r="L10" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="L10" s="21" t="s">
+      <c r="M10" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="M10" s="21" t="s">
+      <c r="N10" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="N10" s="21" t="s">
+      <c r="O10" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="O10" s="21" t="s">
+      <c r="P10" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="P10" s="21" t="s">
+      <c r="Q10" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="Q10" s="21" t="s">
+      <c r="R10" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="R10" s="21" t="s">
+      <c r="S10" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="S10" s="21" t="s">
+      <c r="T10" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="T10" s="21" t="s">
+      <c r="U10" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="U10" s="21" t="s">
+      <c r="V10" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="V10" s="21" t="s">
+      <c r="W10" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="W10" s="21" t="s">
+      <c r="X10" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="X10" s="21" t="s">
+      <c r="Y10" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="Y10" s="21" t="s">
+      <c r="Z10" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="Z10" s="21" t="s">
+      <c r="AA10" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="AA10" s="21" t="s">
+      <c r="AB10" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="AB10" s="21" t="s">
+      <c r="AC10" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="AC10" s="21" t="s">
+      <c r="AD10" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="AD10" s="21" t="s">
+    </row>
+    <row r="11" spans="1:57" ht="88.5">
+      <c r="A11" s="58" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="11" spans="1:57" ht="84">
-      <c r="A11" s="36" t="s">
+      <c r="B11" s="59"/>
+      <c r="C11" s="74" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="23" t="s">
+      <c r="D11" s="74" t="s">
         <v>74</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="E11" s="74" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="F11" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="G11" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="H11" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="I11" s="74" t="s">
+        <v>73</v>
+      </c>
+      <c r="J11" s="74" t="s">
         <v>79</v>
       </c>
-      <c r="I11" s="23" t="s">
+      <c r="K11" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="J11" s="23" t="s">
+      <c r="L11" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K11" s="21" t="s">
+      <c r="M11" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="L11" s="21" t="s">
+      <c r="N11" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="M11" s="21" t="s">
+      <c r="O11" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="N11" s="21" t="s">
+      <c r="P11" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="O11" s="21" t="s">
+      <c r="Q11" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="P11" s="21" t="s">
+      <c r="R11" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="Q11" s="21" t="s">
+      <c r="S11" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="R11" s="21" t="s">
+      <c r="T11" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="S11" s="31" t="s">
+      <c r="U11" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="T11" s="21" t="s">
+      <c r="V11" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="U11" s="21" t="s">
+      <c r="W11" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="V11" s="21" t="s">
+      <c r="X11" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="W11" s="21" t="s">
+      <c r="Y11" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="X11" s="21" t="s">
+      <c r="Z11" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="Y11" s="23" t="s">
+      <c r="AA11" s="74" t="s">
         <v>96</v>
       </c>
-      <c r="Z11" s="23" t="s">
+      <c r="AB11" s="74" t="s">
         <v>97</v>
       </c>
-      <c r="AA11" s="23" t="s">
+      <c r="AC11" s="74" t="s">
         <v>98</v>
       </c>
-      <c r="AB11" s="23" t="s">
+      <c r="AD11" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="AC11" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="AD11" s="23"/>
     </row>
     <row r="12" spans="1:57">
       <c r="A12" s="9"/>
@@ -3339,89 +3349,89 @@
       <c r="AB13" s="6"/>
       <c r="AC13" s="7"/>
       <c r="AD13" s="7"/>
-      <c r="AE13" s="55" t="s">
+      <c r="AE13" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF13" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="AF13" s="57" t="s">
+      <c r="AG13" s="47"/>
+      <c r="AH13" s="47"/>
+      <c r="AI13" s="47"/>
+      <c r="AJ13" s="47"/>
+      <c r="AK13" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL13" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="AG13" s="57"/>
-      <c r="AH13" s="57"/>
-      <c r="AI13" s="57"/>
-      <c r="AJ13" s="57"/>
-      <c r="AK13" s="59" t="s">
-        <v>73</v>
-      </c>
-      <c r="AL13" s="53" t="s">
-        <v>103</v>
-      </c>
-      <c r="AM13" s="53"/>
-      <c r="AN13" s="53"/>
-      <c r="AO13" s="54"/>
+      <c r="AM13" s="50"/>
+      <c r="AN13" s="50"/>
+      <c r="AO13" s="51"/>
       <c r="AP13" s="7"/>
       <c r="AQ13" s="7"/>
       <c r="AR13" s="7"/>
-      <c r="AS13" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="AT13" s="60" t="s">
-        <v>104</v>
-      </c>
-      <c r="AU13" s="60"/>
-      <c r="AV13" s="60"/>
-      <c r="AW13" s="60"/>
-      <c r="AX13" s="60"/>
-      <c r="AY13" s="60"/>
-      <c r="AZ13" s="60"/>
-      <c r="BA13" s="59" t="s">
-        <v>73</v>
-      </c>
-      <c r="BB13" s="53" t="s">
+      <c r="AS13" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="AT13" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="BC13" s="53"/>
-      <c r="BD13" s="53"/>
-      <c r="BE13" s="54"/>
+      <c r="AU13" s="52"/>
+      <c r="AV13" s="52"/>
+      <c r="AW13" s="52"/>
+      <c r="AX13" s="52"/>
+      <c r="AY13" s="52"/>
+      <c r="AZ13" s="52"/>
+      <c r="BA13" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="BB13" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="BC13" s="50"/>
+      <c r="BD13" s="50"/>
+      <c r="BE13" s="51"/>
     </row>
     <row r="14" spans="1:57" ht="15.75">
       <c r="AB14" s="6"/>
       <c r="AC14" s="7"/>
       <c r="AD14" s="7"/>
-      <c r="AE14" s="56"/>
-      <c r="AF14" s="58"/>
-      <c r="AG14" s="58"/>
-      <c r="AH14" s="58"/>
-      <c r="AI14" s="58"/>
-      <c r="AJ14" s="58"/>
-      <c r="AK14" s="56"/>
-      <c r="AL14" s="53" t="s">
+      <c r="AE14" s="46"/>
+      <c r="AF14" s="48"/>
+      <c r="AG14" s="48"/>
+      <c r="AH14" s="48"/>
+      <c r="AI14" s="48"/>
+      <c r="AJ14" s="48"/>
+      <c r="AK14" s="46"/>
+      <c r="AL14" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM14" s="51"/>
+      <c r="AN14" s="53" t="s">
         <v>105</v>
       </c>
-      <c r="AM14" s="54"/>
-      <c r="AN14" s="52" t="s">
-        <v>106</v>
-      </c>
-      <c r="AO14" s="54"/>
+      <c r="AO14" s="51"/>
       <c r="AP14" s="7"/>
       <c r="AQ14" s="7"/>
       <c r="AR14" s="7"/>
-      <c r="AS14" s="56"/>
-      <c r="AT14" s="56"/>
-      <c r="AU14" s="56"/>
-      <c r="AV14" s="56"/>
-      <c r="AW14" s="56"/>
-      <c r="AX14" s="56"/>
-      <c r="AY14" s="56"/>
-      <c r="AZ14" s="56"/>
-      <c r="BA14" s="56"/>
-      <c r="BB14" s="53" t="s">
+      <c r="AS14" s="46"/>
+      <c r="AT14" s="46"/>
+      <c r="AU14" s="46"/>
+      <c r="AV14" s="46"/>
+      <c r="AW14" s="46"/>
+      <c r="AX14" s="46"/>
+      <c r="AY14" s="46"/>
+      <c r="AZ14" s="46"/>
+      <c r="BA14" s="46"/>
+      <c r="BB14" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="BC14" s="51"/>
+      <c r="BD14" s="53" t="s">
         <v>105</v>
       </c>
-      <c r="BC14" s="54"/>
-      <c r="BD14" s="52" t="s">
-        <v>106</v>
-      </c>
-      <c r="BE14" s="54"/>
+      <c r="BE14" s="51"/>
     </row>
     <row r="15" spans="1:57" ht="15.75">
       <c r="AB15" s="1"/>
@@ -3431,27 +3441,27 @@
         <f>IF(AF15&lt;&gt;"",COUNTA($AF$15:AF15),"")</f>
         <v>1</v>
       </c>
-      <c r="AF15" s="61" t="s">
-        <v>107</v>
-      </c>
-      <c r="AG15" s="62"/>
-      <c r="AH15" s="62"/>
-      <c r="AI15" s="62"/>
-      <c r="AJ15" s="62"/>
+      <c r="AF15" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG15" s="37"/>
+      <c r="AH15" s="37"/>
+      <c r="AI15" s="37"/>
+      <c r="AJ15" s="37"/>
       <c r="AK15" s="3" t="e">
         <f>COUNTIF([1]!Danhsachchung[Đơn vị cũ],AF15)</f>
         <v>#REF!</v>
       </c>
-      <c r="AL15" s="63" t="e">
+      <c r="AL15" s="38" t="e">
         <f>COUNTIF([1]KCL1!$H$3:H100,AF15)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AM15" s="64"/>
-      <c r="AN15" s="63" t="e">
+      <c r="AM15" s="39"/>
+      <c r="AN15" s="38" t="e">
         <f>COUNTIF([1]K1!$H$3:J100,AF15)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AO15" s="64"/>
+      <c r="AO15" s="39"/>
       <c r="AP15" s="5"/>
       <c r="AQ15" s="5"/>
       <c r="AR15" s="5"/>
@@ -3459,29 +3469,29 @@
         <f>IF(AT15&lt;&gt;"",(COUNTA($AF$15:AF31)+COUNTA($AT$15:AT15)),"")</f>
         <v>18</v>
       </c>
-      <c r="AT15" s="61" t="s">
-        <v>108</v>
-      </c>
-      <c r="AU15" s="62"/>
-      <c r="AV15" s="62"/>
-      <c r="AW15" s="62"/>
-      <c r="AX15" s="62"/>
-      <c r="AY15" s="62"/>
-      <c r="AZ15" s="65"/>
-      <c r="BA15" s="27" t="e">
+      <c r="AT15" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="AU15" s="37"/>
+      <c r="AV15" s="37"/>
+      <c r="AW15" s="37"/>
+      <c r="AX15" s="37"/>
+      <c r="AY15" s="37"/>
+      <c r="AZ15" s="43"/>
+      <c r="BA15" s="31" t="e">
         <f>COUNTIF([1]!Danhsachchung[Đơn vị cũ],AT15)</f>
         <v>#REF!</v>
       </c>
-      <c r="BB15" s="63" t="e">
+      <c r="BB15" s="38" t="e">
         <f>COUNTIF([1]KCL1!$H$3:$H$100,AT15)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BC15" s="64"/>
-      <c r="BD15" s="63" t="e">
+      <c r="BC15" s="39"/>
+      <c r="BD15" s="38" t="e">
         <f>COUNTIF([1]K1!$H$3:$H$100,AT15)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BE15" s="64"/>
+      <c r="BE15" s="39"/>
     </row>
     <row r="16" spans="1:57" ht="15.75">
       <c r="AB16" s="1"/>
@@ -3491,27 +3501,27 @@
         <f>IF(AF16&lt;&gt;"",COUNTA($AF$15:AF16),"")</f>
         <v>2</v>
       </c>
-      <c r="AF16" s="61" t="s">
-        <v>109</v>
-      </c>
-      <c r="AG16" s="62"/>
-      <c r="AH16" s="62"/>
-      <c r="AI16" s="62"/>
-      <c r="AJ16" s="62"/>
+      <c r="AF16" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="AG16" s="37"/>
+      <c r="AH16" s="37"/>
+      <c r="AI16" s="37"/>
+      <c r="AJ16" s="37"/>
       <c r="AK16" s="3" t="e">
         <f>COUNTIF([1]!Danhsachchung[Đơn vị cũ],AF16)</f>
         <v>#REF!</v>
       </c>
-      <c r="AL16" s="63" t="e">
+      <c r="AL16" s="38" t="e">
         <f>COUNTIF([1]KCL1!$H$3:H101,AF16)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AM16" s="64"/>
-      <c r="AN16" s="63" t="e">
+      <c r="AM16" s="39"/>
+      <c r="AN16" s="38" t="e">
         <f>COUNTIF([1]K1!$H$3:J101,AF16)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AO16" s="64"/>
+      <c r="AO16" s="39"/>
       <c r="AP16" s="5"/>
       <c r="AQ16" s="5"/>
       <c r="AR16" s="5"/>
@@ -3519,29 +3529,29 @@
         <f>IF(AT16&lt;&gt;"",(COUNTA($B$15:B32)+COUNTA($AT$15:AT16)),"")</f>
         <v>2</v>
       </c>
-      <c r="AT16" s="61" t="s">
-        <v>110</v>
-      </c>
-      <c r="AU16" s="62"/>
-      <c r="AV16" s="62"/>
-      <c r="AW16" s="62"/>
-      <c r="AX16" s="62"/>
-      <c r="AY16" s="62"/>
-      <c r="AZ16" s="62"/>
-      <c r="BA16" s="27" t="e">
+      <c r="AT16" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="AU16" s="37"/>
+      <c r="AV16" s="37"/>
+      <c r="AW16" s="37"/>
+      <c r="AX16" s="37"/>
+      <c r="AY16" s="37"/>
+      <c r="AZ16" s="37"/>
+      <c r="BA16" s="31" t="e">
         <f>COUNTIF([1]!Danhsachchung[Đơn vị cũ],AT16)</f>
         <v>#REF!</v>
       </c>
-      <c r="BB16" s="63" t="e">
+      <c r="BB16" s="38" t="e">
         <f>COUNTIF([1]KCL1!$H$3:$H$100,AT16)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BC16" s="64"/>
-      <c r="BD16" s="63" t="e">
+      <c r="BC16" s="39"/>
+      <c r="BD16" s="38" t="e">
         <f>COUNTIF([1]K1!$H$3:$H$100,AT16)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BE16" s="64"/>
+      <c r="BE16" s="39"/>
     </row>
     <row r="17" spans="1:57" ht="15.75">
       <c r="AB17" s="1"/>
@@ -3551,27 +3561,27 @@
         <f>IF(AF17&lt;&gt;"",COUNTA($AF$15:AF17),"")</f>
         <v>3</v>
       </c>
-      <c r="AF17" s="61" t="s">
-        <v>111</v>
-      </c>
-      <c r="AG17" s="62"/>
-      <c r="AH17" s="62"/>
-      <c r="AI17" s="62"/>
-      <c r="AJ17" s="62"/>
+      <c r="AF17" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG17" s="37"/>
+      <c r="AH17" s="37"/>
+      <c r="AI17" s="37"/>
+      <c r="AJ17" s="37"/>
       <c r="AK17" s="3" t="e">
         <f>COUNTIF([1]!Danhsachchung[Đơn vị cũ],AF17)</f>
         <v>#REF!</v>
       </c>
-      <c r="AL17" s="63" t="e">
+      <c r="AL17" s="38" t="e">
         <f>COUNTIF([1]KCL1!$H$3:H102,AF17)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AM17" s="64"/>
-      <c r="AN17" s="63" t="e">
+      <c r="AM17" s="39"/>
+      <c r="AN17" s="38" t="e">
         <f>COUNTIF([1]K1!$H$3:J102,AF17)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AO17" s="64"/>
+      <c r="AO17" s="39"/>
       <c r="AP17" s="5"/>
       <c r="AQ17" s="5"/>
       <c r="AR17" s="5"/>
@@ -3579,29 +3589,29 @@
         <f>IF(AT17&lt;&gt;"",(COUNTA($B$15:B33)+COUNTA($AT$15:AT17)),"")</f>
         <v>3</v>
       </c>
-      <c r="AT17" s="61" t="s">
-        <v>112</v>
-      </c>
-      <c r="AU17" s="62"/>
-      <c r="AV17" s="62"/>
-      <c r="AW17" s="62"/>
-      <c r="AX17" s="62"/>
-      <c r="AY17" s="62"/>
-      <c r="AZ17" s="62"/>
-      <c r="BA17" s="27" t="e">
+      <c r="AT17" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="AU17" s="37"/>
+      <c r="AV17" s="37"/>
+      <c r="AW17" s="37"/>
+      <c r="AX17" s="37"/>
+      <c r="AY17" s="37"/>
+      <c r="AZ17" s="37"/>
+      <c r="BA17" s="31" t="e">
         <f>COUNTIF([1]!Danhsachchung[Đơn vị cũ],AT17)</f>
         <v>#REF!</v>
       </c>
-      <c r="BB17" s="63" t="e">
+      <c r="BB17" s="38" t="e">
         <f>COUNTIF([1]KCL1!$H$3:$H$100,AT17)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BC17" s="64"/>
-      <c r="BD17" s="63" t="e">
+      <c r="BC17" s="39"/>
+      <c r="BD17" s="38" t="e">
         <f>COUNTIF([1]K1!$H$3:$H$100,AT17)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BE17" s="64"/>
+      <c r="BE17" s="39"/>
     </row>
     <row r="18" spans="1:57" ht="15.75">
       <c r="AB18" s="1"/>
@@ -3611,27 +3621,27 @@
         <f>IF(AF18&lt;&gt;"",COUNTA($AF$15:AF18),"")</f>
         <v>4</v>
       </c>
-      <c r="AF18" s="61" t="s">
-        <v>113</v>
-      </c>
-      <c r="AG18" s="62"/>
-      <c r="AH18" s="62"/>
-      <c r="AI18" s="62"/>
-      <c r="AJ18" s="62"/>
+      <c r="AF18" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG18" s="37"/>
+      <c r="AH18" s="37"/>
+      <c r="AI18" s="37"/>
+      <c r="AJ18" s="37"/>
       <c r="AK18" s="3" t="e">
         <f>COUNTIF([1]!Danhsachchung[Đơn vị cũ],AF18)</f>
         <v>#REF!</v>
       </c>
-      <c r="AL18" s="63" t="e">
+      <c r="AL18" s="38" t="e">
         <f>COUNTIF([1]KCL1!$H$3:H103,AF18)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AM18" s="64"/>
-      <c r="AN18" s="63" t="e">
+      <c r="AM18" s="39"/>
+      <c r="AN18" s="38" t="e">
         <f>COUNTIF([1]K1!$H$3:J103,AF18)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AO18" s="64"/>
+      <c r="AO18" s="39"/>
       <c r="AP18" s="5"/>
       <c r="AQ18" s="5"/>
       <c r="AR18" s="5"/>
@@ -3639,29 +3649,29 @@
         <f>IF(AT18&lt;&gt;"",(COUNTA($B$15:B34)+COUNTA($AT$15:AT18)),"")</f>
         <v>4</v>
       </c>
-      <c r="AT18" s="61" t="s">
-        <v>114</v>
-      </c>
-      <c r="AU18" s="62"/>
-      <c r="AV18" s="62"/>
-      <c r="AW18" s="62"/>
-      <c r="AX18" s="62"/>
-      <c r="AY18" s="62"/>
-      <c r="AZ18" s="62"/>
-      <c r="BA18" s="27" t="e">
+      <c r="AT18" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="AU18" s="37"/>
+      <c r="AV18" s="37"/>
+      <c r="AW18" s="37"/>
+      <c r="AX18" s="37"/>
+      <c r="AY18" s="37"/>
+      <c r="AZ18" s="37"/>
+      <c r="BA18" s="31" t="e">
         <f>COUNTIF([1]!Danhsachchung[Đơn vị cũ],AT18)</f>
         <v>#REF!</v>
       </c>
-      <c r="BB18" s="63" t="e">
+      <c r="BB18" s="38" t="e">
         <f>COUNTIF([1]KCL1!$H$3:$H$100,AT18)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BC18" s="64"/>
-      <c r="BD18" s="63" t="e">
+      <c r="BC18" s="39"/>
+      <c r="BD18" s="38" t="e">
         <f>COUNTIF([1]K1!$H$3:$H$100,AT18)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BE18" s="64"/>
+      <c r="BE18" s="39"/>
     </row>
     <row r="19" spans="1:57" ht="15.75">
       <c r="AB19" s="1"/>
@@ -3671,27 +3681,27 @@
         <f>IF(AF19&lt;&gt;"",COUNTA($AF$15:AF19),"")</f>
         <v>5</v>
       </c>
-      <c r="AF19" s="61" t="s">
-        <v>115</v>
-      </c>
-      <c r="AG19" s="62"/>
-      <c r="AH19" s="62"/>
-      <c r="AI19" s="62"/>
-      <c r="AJ19" s="62"/>
+      <c r="AF19" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG19" s="37"/>
+      <c r="AH19" s="37"/>
+      <c r="AI19" s="37"/>
+      <c r="AJ19" s="37"/>
       <c r="AK19" s="3" t="e">
         <f>COUNTIF([1]!Danhsachchung[Đơn vị cũ],AF19)</f>
         <v>#REF!</v>
       </c>
-      <c r="AL19" s="63" t="e">
+      <c r="AL19" s="38" t="e">
         <f>COUNTIF([1]KCL1!$H$3:H104,AF19)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AM19" s="64"/>
-      <c r="AN19" s="63" t="e">
+      <c r="AM19" s="39"/>
+      <c r="AN19" s="38" t="e">
         <f>COUNTIF([1]K1!$H$3:J104,AF19)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AO19" s="64"/>
+      <c r="AO19" s="39"/>
       <c r="AP19" s="5"/>
       <c r="AQ19" s="5"/>
       <c r="AR19" s="5"/>
@@ -3699,27 +3709,27 @@
         <f>IF(AT19&lt;&gt;"",(COUNTA($B$15:B35)+COUNTA($AT$15:AT19)),"")</f>
         <v/>
       </c>
-      <c r="AT19" s="61"/>
-      <c r="AU19" s="62"/>
-      <c r="AV19" s="62"/>
-      <c r="AW19" s="62"/>
-      <c r="AX19" s="62"/>
-      <c r="AY19" s="62"/>
-      <c r="AZ19" s="62"/>
-      <c r="BA19" s="27" t="e">
+      <c r="AT19" s="36"/>
+      <c r="AU19" s="37"/>
+      <c r="AV19" s="37"/>
+      <c r="AW19" s="37"/>
+      <c r="AX19" s="37"/>
+      <c r="AY19" s="37"/>
+      <c r="AZ19" s="37"/>
+      <c r="BA19" s="31" t="e">
         <f>COUNTIF([1]!Danhsachchung[Đơn vị cũ],AT19)</f>
         <v>#REF!</v>
       </c>
-      <c r="BB19" s="63" t="e">
+      <c r="BB19" s="38" t="e">
         <f>COUNTIF([1]KCL1!$H$3:$H$100,AT19)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BC19" s="64"/>
-      <c r="BD19" s="63" t="e">
+      <c r="BC19" s="39"/>
+      <c r="BD19" s="38" t="e">
         <f>COUNTIF([1]K1!$H$3:$H$100,AT19)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BE19" s="64"/>
+      <c r="BE19" s="39"/>
     </row>
     <row r="20" spans="1:57" ht="15.75">
       <c r="AB20" s="1"/>
@@ -3729,27 +3739,27 @@
         <f>IF(AF20&lt;&gt;"",COUNTA($AF$15:AF20),"")</f>
         <v>6</v>
       </c>
-      <c r="AF20" s="61" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG20" s="62"/>
-      <c r="AH20" s="62"/>
-      <c r="AI20" s="62"/>
-      <c r="AJ20" s="62"/>
+      <c r="AF20" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG20" s="37"/>
+      <c r="AH20" s="37"/>
+      <c r="AI20" s="37"/>
+      <c r="AJ20" s="37"/>
       <c r="AK20" s="3" t="e">
         <f>COUNTIF([1]!Danhsachchung[Đơn vị cũ],AF20)</f>
         <v>#REF!</v>
       </c>
-      <c r="AL20" s="63" t="e">
+      <c r="AL20" s="38" t="e">
         <f>COUNTIF([1]KCL1!$H$3:H105,AF20)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AM20" s="64"/>
-      <c r="AN20" s="63" t="e">
+      <c r="AM20" s="39"/>
+      <c r="AN20" s="38" t="e">
         <f>COUNTIF([1]K1!$H$3:J105,AF20)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AO20" s="64"/>
+      <c r="AO20" s="39"/>
       <c r="AP20" s="5"/>
       <c r="AQ20" s="5"/>
       <c r="AR20" s="5"/>
@@ -3757,18 +3767,18 @@
         <f>IF(AT20&lt;&gt;"",(COUNTA($B$15:B36)+COUNTA($AT$15:AT20)),"")</f>
         <v/>
       </c>
-      <c r="AT20" s="61"/>
-      <c r="AU20" s="62"/>
-      <c r="AV20" s="62"/>
-      <c r="AW20" s="62"/>
-      <c r="AX20" s="62"/>
-      <c r="AY20" s="62"/>
-      <c r="AZ20" s="65"/>
-      <c r="BA20" s="27"/>
-      <c r="BB20" s="63"/>
-      <c r="BC20" s="64"/>
-      <c r="BD20" s="66"/>
-      <c r="BE20" s="64"/>
+      <c r="AT20" s="36"/>
+      <c r="AU20" s="37"/>
+      <c r="AV20" s="37"/>
+      <c r="AW20" s="37"/>
+      <c r="AX20" s="37"/>
+      <c r="AY20" s="37"/>
+      <c r="AZ20" s="43"/>
+      <c r="BA20" s="31"/>
+      <c r="BB20" s="38"/>
+      <c r="BC20" s="39"/>
+      <c r="BD20" s="44"/>
+      <c r="BE20" s="39"/>
     </row>
     <row r="21" spans="1:57" ht="15.75">
       <c r="AB21" s="1"/>
@@ -3778,27 +3788,27 @@
         <f>IF(AF21&lt;&gt;"",COUNTA($AF$15:AF21),"")</f>
         <v>7</v>
       </c>
-      <c r="AF21" s="61" t="s">
-        <v>117</v>
-      </c>
-      <c r="AG21" s="62"/>
-      <c r="AH21" s="62"/>
-      <c r="AI21" s="62"/>
-      <c r="AJ21" s="62"/>
+      <c r="AF21" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG21" s="37"/>
+      <c r="AH21" s="37"/>
+      <c r="AI21" s="37"/>
+      <c r="AJ21" s="37"/>
       <c r="AK21" s="3" t="e">
         <f>COUNTIF([1]!Danhsachchung[Đơn vị cũ],AF21)</f>
         <v>#REF!</v>
       </c>
-      <c r="AL21" s="63" t="e">
+      <c r="AL21" s="38" t="e">
         <f>COUNTIF([1]KCL1!$H$3:H106,AF21)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AM21" s="64"/>
-      <c r="AN21" s="63" t="e">
+      <c r="AM21" s="39"/>
+      <c r="AN21" s="38" t="e">
         <f>COUNTIF([1]K1!$H$3:J106,AF21)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AO21" s="64"/>
+      <c r="AO21" s="39"/>
       <c r="AP21" s="5"/>
       <c r="AQ21" s="5"/>
       <c r="AR21" s="5"/>
@@ -3806,18 +3816,18 @@
         <f>IF(AT21&lt;&gt;"",(COUNTA($B$15:B37)+COUNTA($AT$15:AT21)),"")</f>
         <v/>
       </c>
-      <c r="AT21" s="61"/>
-      <c r="AU21" s="62"/>
-      <c r="AV21" s="62"/>
-      <c r="AW21" s="62"/>
-      <c r="AX21" s="62"/>
-      <c r="AY21" s="62"/>
-      <c r="AZ21" s="65"/>
-      <c r="BA21" s="27"/>
-      <c r="BB21" s="63"/>
-      <c r="BC21" s="64"/>
-      <c r="BD21" s="66"/>
-      <c r="BE21" s="64"/>
+      <c r="AT21" s="36"/>
+      <c r="AU21" s="37"/>
+      <c r="AV21" s="37"/>
+      <c r="AW21" s="37"/>
+      <c r="AX21" s="37"/>
+      <c r="AY21" s="37"/>
+      <c r="AZ21" s="43"/>
+      <c r="BA21" s="31"/>
+      <c r="BB21" s="38"/>
+      <c r="BC21" s="39"/>
+      <c r="BD21" s="44"/>
+      <c r="BE21" s="39"/>
     </row>
     <row r="22" spans="1:57" ht="15.75">
       <c r="AB22" s="1"/>
@@ -3827,27 +3837,27 @@
         <f>IF(AF22&lt;&gt;"",COUNTA($AF$15:AF22),"")</f>
         <v>8</v>
       </c>
-      <c r="AF22" s="61" t="s">
-        <v>118</v>
-      </c>
-      <c r="AG22" s="62"/>
-      <c r="AH22" s="62"/>
-      <c r="AI22" s="62"/>
-      <c r="AJ22" s="62"/>
+      <c r="AF22" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG22" s="37"/>
+      <c r="AH22" s="37"/>
+      <c r="AI22" s="37"/>
+      <c r="AJ22" s="37"/>
       <c r="AK22" s="3" t="e">
         <f>COUNTIF([1]!Danhsachchung[Đơn vị cũ],AF22)</f>
         <v>#REF!</v>
       </c>
-      <c r="AL22" s="63" t="e">
+      <c r="AL22" s="38" t="e">
         <f>COUNTIF([1]KCL1!$H$3:H107,AF22)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AM22" s="64"/>
-      <c r="AN22" s="63" t="e">
+      <c r="AM22" s="39"/>
+      <c r="AN22" s="38" t="e">
         <f>COUNTIF([1]K1!$H$3:J107,AF22)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AO22" s="64"/>
+      <c r="AO22" s="39"/>
       <c r="AP22" s="5"/>
       <c r="AQ22" s="5"/>
       <c r="AR22" s="5"/>
@@ -3855,18 +3865,18 @@
         <f>IF(AT22&lt;&gt;"",(COUNTA($B$15:B38)+COUNTA($AT$15:AT22)),"")</f>
         <v/>
       </c>
-      <c r="AT22" s="61"/>
-      <c r="AU22" s="62"/>
-      <c r="AV22" s="62"/>
-      <c r="AW22" s="62"/>
-      <c r="AX22" s="62"/>
-      <c r="AY22" s="62"/>
-      <c r="AZ22" s="65"/>
-      <c r="BA22" s="27"/>
-      <c r="BB22" s="63"/>
-      <c r="BC22" s="64"/>
-      <c r="BD22" s="66"/>
-      <c r="BE22" s="64"/>
+      <c r="AT22" s="36"/>
+      <c r="AU22" s="37"/>
+      <c r="AV22" s="37"/>
+      <c r="AW22" s="37"/>
+      <c r="AX22" s="37"/>
+      <c r="AY22" s="37"/>
+      <c r="AZ22" s="43"/>
+      <c r="BA22" s="31"/>
+      <c r="BB22" s="38"/>
+      <c r="BC22" s="39"/>
+      <c r="BD22" s="44"/>
+      <c r="BE22" s="39"/>
     </row>
     <row r="23" spans="1:57" ht="15.75">
       <c r="AB23" s="1"/>
@@ -3876,27 +3886,27 @@
         <f>IF(AF23&lt;&gt;"",COUNTA($AF$15:AF23),"")</f>
         <v>9</v>
       </c>
-      <c r="AF23" s="61" t="s">
-        <v>119</v>
-      </c>
-      <c r="AG23" s="62"/>
-      <c r="AH23" s="62"/>
-      <c r="AI23" s="62"/>
-      <c r="AJ23" s="62"/>
+      <c r="AF23" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="AG23" s="37"/>
+      <c r="AH23" s="37"/>
+      <c r="AI23" s="37"/>
+      <c r="AJ23" s="37"/>
       <c r="AK23" s="3" t="e">
         <f>COUNTIF([1]!Danhsachchung[Đơn vị cũ],AF23)</f>
         <v>#REF!</v>
       </c>
-      <c r="AL23" s="63" t="e">
+      <c r="AL23" s="38" t="e">
         <f>COUNTIF([1]KCL1!$H$3:H108,AF23)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AM23" s="64"/>
-      <c r="AN23" s="63" t="e">
+      <c r="AM23" s="39"/>
+      <c r="AN23" s="38" t="e">
         <f>COUNTIF([1]K1!$H$3:J108,AF23)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AO23" s="64"/>
+      <c r="AO23" s="39"/>
       <c r="AP23" s="5"/>
       <c r="AQ23" s="5"/>
       <c r="AR23" s="5"/>
@@ -3904,18 +3914,18 @@
         <f>IF(AT23&lt;&gt;"",(COUNTA($B$15:B39)+COUNTA($AT$15:AT23)),"")</f>
         <v/>
       </c>
-      <c r="AT23" s="61"/>
-      <c r="AU23" s="62"/>
-      <c r="AV23" s="62"/>
-      <c r="AW23" s="62"/>
-      <c r="AX23" s="62"/>
-      <c r="AY23" s="62"/>
-      <c r="AZ23" s="65"/>
-      <c r="BA23" s="27"/>
-      <c r="BB23" s="63"/>
-      <c r="BC23" s="64"/>
-      <c r="BD23" s="66"/>
-      <c r="BE23" s="64"/>
+      <c r="AT23" s="36"/>
+      <c r="AU23" s="37"/>
+      <c r="AV23" s="37"/>
+      <c r="AW23" s="37"/>
+      <c r="AX23" s="37"/>
+      <c r="AY23" s="37"/>
+      <c r="AZ23" s="43"/>
+      <c r="BA23" s="31"/>
+      <c r="BB23" s="38"/>
+      <c r="BC23" s="39"/>
+      <c r="BD23" s="44"/>
+      <c r="BE23" s="39"/>
     </row>
     <row r="24" spans="1:57" ht="15.75">
       <c r="AB24" s="1"/>
@@ -3925,27 +3935,27 @@
         <f>IF(AF24&lt;&gt;"",COUNTA($AF$15:AF24),"")</f>
         <v>10</v>
       </c>
-      <c r="AF24" s="61" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG24" s="62"/>
-      <c r="AH24" s="62"/>
-      <c r="AI24" s="62"/>
-      <c r="AJ24" s="62"/>
+      <c r="AF24" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="AG24" s="37"/>
+      <c r="AH24" s="37"/>
+      <c r="AI24" s="37"/>
+      <c r="AJ24" s="37"/>
       <c r="AK24" s="3" t="e">
         <f>COUNTIF([1]!Danhsachchung[Đơn vị cũ],AF24)</f>
         <v>#REF!</v>
       </c>
-      <c r="AL24" s="63" t="e">
+      <c r="AL24" s="38" t="e">
         <f>COUNTIF([1]KCL1!$H$3:H109,AF24)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AM24" s="64"/>
-      <c r="AN24" s="63" t="e">
+      <c r="AM24" s="39"/>
+      <c r="AN24" s="38" t="e">
         <f>COUNTIF([1]K1!$H$3:J109,AF24)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AO24" s="64"/>
+      <c r="AO24" s="39"/>
       <c r="AP24" s="5"/>
       <c r="AQ24" s="5"/>
       <c r="AR24" s="5"/>
@@ -3953,18 +3963,18 @@
         <f>IF(AT24&lt;&gt;"",(COUNTA($B$15:B40)+COUNTA($AT$15:AT24)),"")</f>
         <v/>
       </c>
-      <c r="AT24" s="61"/>
-      <c r="AU24" s="62"/>
-      <c r="AV24" s="62"/>
-      <c r="AW24" s="62"/>
-      <c r="AX24" s="62"/>
-      <c r="AY24" s="62"/>
-      <c r="AZ24" s="65"/>
-      <c r="BA24" s="27"/>
-      <c r="BB24" s="63"/>
-      <c r="BC24" s="64"/>
-      <c r="BD24" s="66"/>
-      <c r="BE24" s="64"/>
+      <c r="AT24" s="36"/>
+      <c r="AU24" s="37"/>
+      <c r="AV24" s="37"/>
+      <c r="AW24" s="37"/>
+      <c r="AX24" s="37"/>
+      <c r="AY24" s="37"/>
+      <c r="AZ24" s="43"/>
+      <c r="BA24" s="31"/>
+      <c r="BB24" s="38"/>
+      <c r="BC24" s="39"/>
+      <c r="BD24" s="44"/>
+      <c r="BE24" s="39"/>
     </row>
     <row r="25" spans="1:57" ht="15.75">
       <c r="AB25" s="1"/>
@@ -3974,27 +3984,27 @@
         <f>IF(AF25&lt;&gt;"",COUNTA($AF$15:AF25),"")</f>
         <v>11</v>
       </c>
-      <c r="AF25" s="61" t="s">
-        <v>121</v>
-      </c>
-      <c r="AG25" s="62"/>
-      <c r="AH25" s="62"/>
-      <c r="AI25" s="62"/>
-      <c r="AJ25" s="62"/>
+      <c r="AF25" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG25" s="37"/>
+      <c r="AH25" s="37"/>
+      <c r="AI25" s="37"/>
+      <c r="AJ25" s="37"/>
       <c r="AK25" s="3" t="e">
         <f>COUNTIF([1]!Danhsachchung[Đơn vị cũ],AF25)</f>
         <v>#REF!</v>
       </c>
-      <c r="AL25" s="63" t="e">
+      <c r="AL25" s="38" t="e">
         <f>COUNTIF([1]KCL1!$H$3:H110,AF25)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AM25" s="64"/>
-      <c r="AN25" s="63" t="e">
+      <c r="AM25" s="39"/>
+      <c r="AN25" s="38" t="e">
         <f>COUNTIF([1]K1!$H$3:J110,AF25)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AO25" s="64"/>
+      <c r="AO25" s="39"/>
       <c r="AP25" s="5"/>
       <c r="AQ25" s="5"/>
       <c r="AR25" s="5"/>
@@ -4002,18 +4012,18 @@
         <f>IF(AT25&lt;&gt;"",(COUNTA($B$15:B41)+COUNTA($AT$15:AT25)),"")</f>
         <v/>
       </c>
-      <c r="AT25" s="61"/>
-      <c r="AU25" s="62"/>
-      <c r="AV25" s="62"/>
-      <c r="AW25" s="62"/>
-      <c r="AX25" s="62"/>
-      <c r="AY25" s="62"/>
-      <c r="AZ25" s="65"/>
-      <c r="BA25" s="27"/>
-      <c r="BB25" s="63"/>
-      <c r="BC25" s="64"/>
-      <c r="BD25" s="66"/>
-      <c r="BE25" s="64"/>
+      <c r="AT25" s="36"/>
+      <c r="AU25" s="37"/>
+      <c r="AV25" s="37"/>
+      <c r="AW25" s="37"/>
+      <c r="AX25" s="37"/>
+      <c r="AY25" s="37"/>
+      <c r="AZ25" s="43"/>
+      <c r="BA25" s="31"/>
+      <c r="BB25" s="38"/>
+      <c r="BC25" s="39"/>
+      <c r="BD25" s="44"/>
+      <c r="BE25" s="39"/>
     </row>
     <row r="26" spans="1:57" ht="18.75">
       <c r="AB26" s="2"/>
@@ -4023,27 +4033,27 @@
         <f>IF(AF26&lt;&gt;"",COUNTA($AF$15:AF26),"")</f>
         <v>12</v>
       </c>
-      <c r="AF26" s="61" t="s">
-        <v>122</v>
-      </c>
-      <c r="AG26" s="62"/>
-      <c r="AH26" s="62"/>
-      <c r="AI26" s="62"/>
-      <c r="AJ26" s="62"/>
+      <c r="AF26" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG26" s="37"/>
+      <c r="AH26" s="37"/>
+      <c r="AI26" s="37"/>
+      <c r="AJ26" s="37"/>
       <c r="AK26" s="3" t="e">
         <f>COUNTIF([1]!Danhsachchung[Đơn vị cũ],AF26)</f>
         <v>#REF!</v>
       </c>
-      <c r="AL26" s="63" t="e">
+      <c r="AL26" s="38" t="e">
         <f>COUNTIF([1]KCL1!$H$3:H111,AF26)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AM26" s="64"/>
-      <c r="AN26" s="63" t="e">
+      <c r="AM26" s="39"/>
+      <c r="AN26" s="38" t="e">
         <f>COUNTIF([1]K1!$H$3:J111,AF26)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AO26" s="64"/>
+      <c r="AO26" s="39"/>
       <c r="AP26" s="2"/>
       <c r="AQ26" s="1"/>
       <c r="AR26" s="1"/>
@@ -4051,18 +4061,18 @@
         <f>IF(AT26&lt;&gt;"",(COUNTA($B$15:B42)+COUNTA($AT$15:AT26)),"")</f>
         <v/>
       </c>
-      <c r="AT26" s="61"/>
-      <c r="AU26" s="62"/>
-      <c r="AV26" s="62"/>
-      <c r="AW26" s="62"/>
-      <c r="AX26" s="62"/>
-      <c r="AY26" s="62"/>
-      <c r="AZ26" s="65"/>
-      <c r="BA26" s="27"/>
-      <c r="BB26" s="63"/>
-      <c r="BC26" s="64"/>
-      <c r="BD26" s="66"/>
-      <c r="BE26" s="64"/>
+      <c r="AT26" s="36"/>
+      <c r="AU26" s="37"/>
+      <c r="AV26" s="37"/>
+      <c r="AW26" s="37"/>
+      <c r="AX26" s="37"/>
+      <c r="AY26" s="37"/>
+      <c r="AZ26" s="43"/>
+      <c r="BA26" s="31"/>
+      <c r="BB26" s="38"/>
+      <c r="BC26" s="39"/>
+      <c r="BD26" s="44"/>
+      <c r="BE26" s="39"/>
     </row>
     <row r="27" spans="1:57" ht="18.75">
       <c r="AB27" s="2"/>
@@ -4072,27 +4082,27 @@
         <f>IF(AF27&lt;&gt;"",COUNTA($AF$15:AF27),"")</f>
         <v>13</v>
       </c>
-      <c r="AF27" s="61" t="s">
-        <v>123</v>
-      </c>
-      <c r="AG27" s="62"/>
-      <c r="AH27" s="62"/>
-      <c r="AI27" s="62"/>
-      <c r="AJ27" s="62"/>
+      <c r="AF27" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG27" s="37"/>
+      <c r="AH27" s="37"/>
+      <c r="AI27" s="37"/>
+      <c r="AJ27" s="37"/>
       <c r="AK27" s="3" t="e">
         <f>COUNTIF([1]!Danhsachchung[Đơn vị cũ],AF27)</f>
         <v>#REF!</v>
       </c>
-      <c r="AL27" s="63" t="e">
+      <c r="AL27" s="38" t="e">
         <f>COUNTIF([1]KCL1!$H$3:H112,AF27)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AM27" s="64"/>
-      <c r="AN27" s="63" t="e">
+      <c r="AM27" s="39"/>
+      <c r="AN27" s="38" t="e">
         <f>COUNTIF([1]K1!$H$3:J112,AF27)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AO27" s="64"/>
+      <c r="AO27" s="39"/>
       <c r="AP27" s="2"/>
       <c r="AQ27" s="1"/>
       <c r="AR27" s="1"/>
@@ -4100,18 +4110,18 @@
         <f>IF(AT27&lt;&gt;"",(COUNTA($B$15:B43)+COUNTA($AT$15:AT27)),"")</f>
         <v/>
       </c>
-      <c r="AT27" s="61"/>
-      <c r="AU27" s="62"/>
-      <c r="AV27" s="62"/>
-      <c r="AW27" s="62"/>
-      <c r="AX27" s="62"/>
-      <c r="AY27" s="62"/>
-      <c r="AZ27" s="65"/>
-      <c r="BA27" s="27"/>
-      <c r="BB27" s="63"/>
-      <c r="BC27" s="64"/>
-      <c r="BD27" s="66"/>
-      <c r="BE27" s="64"/>
+      <c r="AT27" s="36"/>
+      <c r="AU27" s="37"/>
+      <c r="AV27" s="37"/>
+      <c r="AW27" s="37"/>
+      <c r="AX27" s="37"/>
+      <c r="AY27" s="37"/>
+      <c r="AZ27" s="43"/>
+      <c r="BA27" s="31"/>
+      <c r="BB27" s="38"/>
+      <c r="BC27" s="39"/>
+      <c r="BD27" s="44"/>
+      <c r="BE27" s="39"/>
     </row>
     <row r="28" spans="1:57" ht="18.75">
       <c r="AB28" s="2"/>
@@ -4121,27 +4131,27 @@
         <f>IF(AF28&lt;&gt;"",COUNTA($AF$15:AF28),"")</f>
         <v>14</v>
       </c>
-      <c r="AF28" s="61" t="s">
-        <v>124</v>
-      </c>
-      <c r="AG28" s="62"/>
-      <c r="AH28" s="62"/>
-      <c r="AI28" s="62"/>
-      <c r="AJ28" s="62"/>
+      <c r="AF28" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="AG28" s="37"/>
+      <c r="AH28" s="37"/>
+      <c r="AI28" s="37"/>
+      <c r="AJ28" s="37"/>
       <c r="AK28" s="3" t="e">
         <f>COUNTIF([1]!Danhsachchung[Đơn vị cũ],AF28)</f>
         <v>#REF!</v>
       </c>
-      <c r="AL28" s="63" t="e">
+      <c r="AL28" s="38" t="e">
         <f>COUNTIF([1]KCL1!$H$3:H113,AF28)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AM28" s="64"/>
-      <c r="AN28" s="63" t="e">
+      <c r="AM28" s="39"/>
+      <c r="AN28" s="38" t="e">
         <f>COUNTIF([1]K1!$H$3:J113,AF28)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AO28" s="64"/>
+      <c r="AO28" s="39"/>
       <c r="AP28" s="2"/>
       <c r="AQ28" s="1"/>
       <c r="AR28" s="1"/>
@@ -4149,18 +4159,18 @@
         <f>IF(AT28&lt;&gt;"",(COUNTA($B$15:B44)+COUNTA($AT$15:AT28)),"")</f>
         <v/>
       </c>
-      <c r="AT28" s="61"/>
-      <c r="AU28" s="62"/>
-      <c r="AV28" s="62"/>
-      <c r="AW28" s="62"/>
-      <c r="AX28" s="62"/>
-      <c r="AY28" s="62"/>
-      <c r="AZ28" s="65"/>
-      <c r="BA28" s="27"/>
-      <c r="BB28" s="63"/>
-      <c r="BC28" s="64"/>
-      <c r="BD28" s="66"/>
-      <c r="BE28" s="64"/>
+      <c r="AT28" s="36"/>
+      <c r="AU28" s="37"/>
+      <c r="AV28" s="37"/>
+      <c r="AW28" s="37"/>
+      <c r="AX28" s="37"/>
+      <c r="AY28" s="37"/>
+      <c r="AZ28" s="43"/>
+      <c r="BA28" s="31"/>
+      <c r="BB28" s="38"/>
+      <c r="BC28" s="39"/>
+      <c r="BD28" s="44"/>
+      <c r="BE28" s="39"/>
     </row>
     <row r="29" spans="1:57" ht="18.75">
       <c r="AB29" s="2"/>
@@ -4170,27 +4180,27 @@
         <f>IF(AF29&lt;&gt;"",COUNTA($AF$15:AF29),"")</f>
         <v>15</v>
       </c>
-      <c r="AF29" s="61" t="s">
-        <v>125</v>
-      </c>
-      <c r="AG29" s="62"/>
-      <c r="AH29" s="62"/>
-      <c r="AI29" s="62"/>
-      <c r="AJ29" s="62"/>
+      <c r="AF29" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="AG29" s="37"/>
+      <c r="AH29" s="37"/>
+      <c r="AI29" s="37"/>
+      <c r="AJ29" s="37"/>
       <c r="AK29" s="3" t="e">
         <f>COUNTIF([1]!Danhsachchung[Đơn vị cũ],AF29)</f>
         <v>#REF!</v>
       </c>
-      <c r="AL29" s="63" t="e">
+      <c r="AL29" s="38" t="e">
         <f>COUNTIF([1]KCL1!$H$3:H114,AF29)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AM29" s="64"/>
-      <c r="AN29" s="63" t="e">
+      <c r="AM29" s="39"/>
+      <c r="AN29" s="38" t="e">
         <f>COUNTIF([1]K1!$H$3:J114,AF29)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AO29" s="64"/>
+      <c r="AO29" s="39"/>
       <c r="AP29" s="2"/>
       <c r="AQ29" s="1"/>
       <c r="AR29" s="1"/>
@@ -4198,18 +4208,18 @@
         <f>IF(AT29&lt;&gt;"",(COUNTA($B$15:B45)+COUNTA($AT$15:AT29)),"")</f>
         <v/>
       </c>
-      <c r="AT29" s="61"/>
-      <c r="AU29" s="62"/>
-      <c r="AV29" s="62"/>
-      <c r="AW29" s="62"/>
-      <c r="AX29" s="62"/>
-      <c r="AY29" s="62"/>
-      <c r="AZ29" s="65"/>
-      <c r="BA29" s="27"/>
-      <c r="BB29" s="63"/>
-      <c r="BC29" s="64"/>
-      <c r="BD29" s="66"/>
-      <c r="BE29" s="64"/>
+      <c r="AT29" s="36"/>
+      <c r="AU29" s="37"/>
+      <c r="AV29" s="37"/>
+      <c r="AW29" s="37"/>
+      <c r="AX29" s="37"/>
+      <c r="AY29" s="37"/>
+      <c r="AZ29" s="43"/>
+      <c r="BA29" s="31"/>
+      <c r="BB29" s="38"/>
+      <c r="BC29" s="39"/>
+      <c r="BD29" s="44"/>
+      <c r="BE29" s="39"/>
     </row>
     <row r="30" spans="1:57" ht="18.75">
       <c r="AB30" s="2"/>
@@ -4219,27 +4229,27 @@
         <f>IF(AF30&lt;&gt;"",COUNTA($AF$15:AF30),"")</f>
         <v>16</v>
       </c>
-      <c r="AF30" s="61" t="s">
-        <v>126</v>
-      </c>
-      <c r="AG30" s="62"/>
-      <c r="AH30" s="62"/>
-      <c r="AI30" s="62"/>
-      <c r="AJ30" s="62"/>
+      <c r="AF30" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="AG30" s="37"/>
+      <c r="AH30" s="37"/>
+      <c r="AI30" s="37"/>
+      <c r="AJ30" s="37"/>
       <c r="AK30" s="3" t="e">
         <f>COUNTIF([1]!Danhsachchung[Đơn vị cũ],AF30)</f>
         <v>#REF!</v>
       </c>
-      <c r="AL30" s="63" t="e">
+      <c r="AL30" s="38" t="e">
         <f>COUNTIF([1]KCL1!$H$3:H115,AF30)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AM30" s="64"/>
-      <c r="AN30" s="63" t="e">
+      <c r="AM30" s="39"/>
+      <c r="AN30" s="38" t="e">
         <f>COUNTIF([1]K1!$H$3:J115,AF30)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AO30" s="64"/>
+      <c r="AO30" s="39"/>
       <c r="AP30" s="2"/>
       <c r="AQ30" s="1"/>
       <c r="AR30" s="1"/>
@@ -4247,18 +4257,18 @@
         <f>IF(AT30&lt;&gt;"",(COUNTA($B$15:B46)+COUNTA($AT$15:AT30)),"")</f>
         <v/>
       </c>
-      <c r="AT30" s="61"/>
-      <c r="AU30" s="62"/>
-      <c r="AV30" s="62"/>
-      <c r="AW30" s="62"/>
-      <c r="AX30" s="62"/>
-      <c r="AY30" s="62"/>
-      <c r="AZ30" s="65"/>
-      <c r="BA30" s="27"/>
-      <c r="BB30" s="63"/>
-      <c r="BC30" s="64"/>
-      <c r="BD30" s="66"/>
-      <c r="BE30" s="64"/>
+      <c r="AT30" s="36"/>
+      <c r="AU30" s="37"/>
+      <c r="AV30" s="37"/>
+      <c r="AW30" s="37"/>
+      <c r="AX30" s="37"/>
+      <c r="AY30" s="37"/>
+      <c r="AZ30" s="43"/>
+      <c r="BA30" s="31"/>
+      <c r="BB30" s="38"/>
+      <c r="BC30" s="39"/>
+      <c r="BD30" s="44"/>
+      <c r="BE30" s="39"/>
     </row>
     <row r="31" spans="1:57" ht="18.75">
       <c r="AB31" s="2"/>
@@ -4268,121 +4278,121 @@
         <f>IF(AF31&lt;&gt;"",COUNTA($AF$15:AF31),"")</f>
         <v>17</v>
       </c>
-      <c r="AF31" s="61" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG31" s="62"/>
-      <c r="AH31" s="62"/>
-      <c r="AI31" s="62"/>
-      <c r="AJ31" s="62"/>
+      <c r="AF31" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="AG31" s="37"/>
+      <c r="AH31" s="37"/>
+      <c r="AI31" s="37"/>
+      <c r="AJ31" s="37"/>
       <c r="AK31" s="3" t="e">
         <f>COUNTIF([1]!Danhsachchung[Đơn vị cũ],AF31)</f>
         <v>#REF!</v>
       </c>
-      <c r="AL31" s="63" t="e">
+      <c r="AL31" s="38" t="e">
         <f>COUNTIF([1]KCL1!$H$3:H116,AF31)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AM31" s="64"/>
-      <c r="AN31" s="63" t="e">
+      <c r="AM31" s="39"/>
+      <c r="AN31" s="38" t="e">
         <f>COUNTIF([1]K1!$H$3:J116,AF31)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AO31" s="64"/>
+      <c r="AO31" s="39"/>
       <c r="AP31" s="2"/>
       <c r="AQ31" s="1"/>
       <c r="AR31" s="1"/>
-      <c r="AS31" s="70" t="s">
-        <v>128</v>
-      </c>
-      <c r="AT31" s="71"/>
-      <c r="AU31" s="71"/>
-      <c r="AV31" s="71"/>
-      <c r="AW31" s="71"/>
-      <c r="AX31" s="71"/>
-      <c r="AY31" s="71"/>
-      <c r="AZ31" s="72"/>
+      <c r="AS31" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT31" s="41"/>
+      <c r="AU31" s="41"/>
+      <c r="AV31" s="41"/>
+      <c r="AW31" s="41"/>
+      <c r="AX31" s="41"/>
+      <c r="AY31" s="41"/>
+      <c r="AZ31" s="42"/>
       <c r="BA31" s="25" t="e">
         <f>SUM(AK15:AK31,BA15:BA30)</f>
         <v>#REF!</v>
       </c>
-      <c r="BB31" s="67" t="e">
+      <c r="BB31" s="32" t="e">
         <f>SUM(AL15:AM31,BB15:BC30)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BC31" s="68"/>
-      <c r="BD31" s="67" t="e">
+      <c r="BC31" s="33"/>
+      <c r="BD31" s="32" t="e">
         <f>SUM(AN15:AO31,BD15:BE30)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BE31" s="68"/>
+      <c r="BE31" s="33"/>
     </row>
     <row r="32" spans="1:57">
-      <c r="A32" s="69"/>
-      <c r="B32" s="69"/>
-      <c r="C32" s="69"/>
-      <c r="D32" s="69"/>
-      <c r="E32" s="69"/>
-      <c r="F32" s="69"/>
-      <c r="G32" s="69"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="69"/>
-      <c r="J32" s="69"/>
-      <c r="K32" s="69"/>
-      <c r="L32" s="69"/>
-      <c r="M32" s="69"/>
-      <c r="N32" s="69"/>
-      <c r="O32" s="69"/>
-      <c r="P32" s="69"/>
-      <c r="Q32" s="69"/>
-      <c r="R32" s="69"/>
-      <c r="S32" s="69"/>
-      <c r="T32" s="69"/>
-      <c r="U32" s="69"/>
-      <c r="V32" s="69"/>
-      <c r="W32" s="69"/>
-      <c r="X32" s="69"/>
-      <c r="Y32" s="69"/>
-      <c r="Z32" s="69"/>
-      <c r="AA32" s="69"/>
+      <c r="A32" s="34"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="34"/>
+      <c r="L32" s="34"/>
+      <c r="M32" s="34"/>
+      <c r="N32" s="34"/>
+      <c r="O32" s="34"/>
+      <c r="P32" s="34"/>
+      <c r="Q32" s="34"/>
+      <c r="R32" s="34"/>
+      <c r="S32" s="34"/>
+      <c r="T32" s="34"/>
+      <c r="U32" s="34"/>
+      <c r="V32" s="34"/>
+      <c r="W32" s="34"/>
+      <c r="X32" s="34"/>
+      <c r="Y32" s="34"/>
+      <c r="Z32" s="34"/>
+      <c r="AA32" s="34"/>
       <c r="AB32" s="1"/>
       <c r="AC32" s="1"/>
       <c r="AD32" s="1"/>
     </row>
     <row r="33" spans="1:30">
-      <c r="A33" s="69"/>
-      <c r="B33" s="69"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="69"/>
-      <c r="I33" s="69"/>
-      <c r="J33" s="69"/>
-      <c r="K33" s="69"/>
-      <c r="L33" s="69"/>
-      <c r="M33" s="69"/>
-      <c r="N33" s="69"/>
-      <c r="O33" s="69"/>
-      <c r="P33" s="69"/>
-      <c r="Q33" s="69"/>
-      <c r="R33" s="69"/>
-      <c r="S33" s="69"/>
-      <c r="T33" s="69"/>
-      <c r="U33" s="69"/>
-      <c r="V33" s="69"/>
-      <c r="W33" s="69"/>
-      <c r="X33" s="69"/>
-      <c r="Y33" s="69"/>
-      <c r="Z33" s="69"/>
-      <c r="AA33" s="69"/>
+      <c r="A33" s="34"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="34"/>
+      <c r="L33" s="34"/>
+      <c r="M33" s="34"/>
+      <c r="N33" s="34"/>
+      <c r="O33" s="34"/>
+      <c r="P33" s="34"/>
+      <c r="Q33" s="34"/>
+      <c r="R33" s="34"/>
+      <c r="S33" s="34"/>
+      <c r="T33" s="34"/>
+      <c r="U33" s="34"/>
+      <c r="V33" s="34"/>
+      <c r="W33" s="34"/>
+      <c r="X33" s="34"/>
+      <c r="Y33" s="34"/>
+      <c r="Z33" s="34"/>
+      <c r="AA33" s="34"/>
       <c r="AB33" s="1"/>
       <c r="AC33" s="1"/>
       <c r="AD33" s="1"/>
     </row>
     <row r="34" spans="1:30">
-      <c r="A34" s="26"/>
+      <c r="A34" s="29"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -4394,14 +4404,14 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
-      <c r="M34" s="69"/>
-      <c r="N34" s="69"/>
-      <c r="O34" s="69"/>
-      <c r="P34" s="69"/>
-      <c r="Q34" s="43"/>
-      <c r="R34" s="43"/>
-      <c r="S34" s="43"/>
-      <c r="T34" s="43"/>
+      <c r="M34" s="34"/>
+      <c r="N34" s="34"/>
+      <c r="O34" s="34"/>
+      <c r="P34" s="34"/>
+      <c r="Q34" s="35"/>
+      <c r="R34" s="35"/>
+      <c r="S34" s="35"/>
+      <c r="T34" s="35"/>
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
@@ -4416,125 +4426,6 @@
   </sheetData>
   <sheetProtection formatCells="0"/>
   <mergeCells count="141">
-    <mergeCell ref="BD31:BE31"/>
-    <mergeCell ref="A32:AA32"/>
-    <mergeCell ref="A33:AA33"/>
-    <mergeCell ref="M34:P34"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="S34:T34"/>
-    <mergeCell ref="AF31:AJ31"/>
-    <mergeCell ref="AL31:AM31"/>
-    <mergeCell ref="AN31:AO31"/>
-    <mergeCell ref="AS31:AZ31"/>
-    <mergeCell ref="BB31:BC31"/>
-    <mergeCell ref="AF29:AJ29"/>
-    <mergeCell ref="AL29:AM29"/>
-    <mergeCell ref="AN29:AO29"/>
-    <mergeCell ref="AT29:AZ29"/>
-    <mergeCell ref="BB29:BC29"/>
-    <mergeCell ref="BD29:BE29"/>
-    <mergeCell ref="AF30:AJ30"/>
-    <mergeCell ref="AL30:AM30"/>
-    <mergeCell ref="AN30:AO30"/>
-    <mergeCell ref="AT30:AZ30"/>
-    <mergeCell ref="BB30:BC30"/>
-    <mergeCell ref="BD30:BE30"/>
-    <mergeCell ref="AF27:AJ27"/>
-    <mergeCell ref="AL27:AM27"/>
-    <mergeCell ref="AN27:AO27"/>
-    <mergeCell ref="AT27:AZ27"/>
-    <mergeCell ref="BB27:BC27"/>
-    <mergeCell ref="BD27:BE27"/>
-    <mergeCell ref="AF28:AJ28"/>
-    <mergeCell ref="AL28:AM28"/>
-    <mergeCell ref="AN28:AO28"/>
-    <mergeCell ref="AT28:AZ28"/>
-    <mergeCell ref="BB28:BC28"/>
-    <mergeCell ref="BD28:BE28"/>
-    <mergeCell ref="AF25:AJ25"/>
-    <mergeCell ref="AL25:AM25"/>
-    <mergeCell ref="AN25:AO25"/>
-    <mergeCell ref="AT25:AZ25"/>
-    <mergeCell ref="BB25:BC25"/>
-    <mergeCell ref="BD25:BE25"/>
-    <mergeCell ref="AF26:AJ26"/>
-    <mergeCell ref="AL26:AM26"/>
-    <mergeCell ref="AN26:AO26"/>
-    <mergeCell ref="AT26:AZ26"/>
-    <mergeCell ref="BB26:BC26"/>
-    <mergeCell ref="BD26:BE26"/>
-    <mergeCell ref="AF23:AJ23"/>
-    <mergeCell ref="AL23:AM23"/>
-    <mergeCell ref="AN23:AO23"/>
-    <mergeCell ref="AT23:AZ23"/>
-    <mergeCell ref="BB23:BC23"/>
-    <mergeCell ref="BD23:BE23"/>
-    <mergeCell ref="AF24:AJ24"/>
-    <mergeCell ref="AL24:AM24"/>
-    <mergeCell ref="AN24:AO24"/>
-    <mergeCell ref="AT24:AZ24"/>
-    <mergeCell ref="BB24:BC24"/>
-    <mergeCell ref="BD24:BE24"/>
-    <mergeCell ref="AF21:AJ21"/>
-    <mergeCell ref="AL21:AM21"/>
-    <mergeCell ref="AN21:AO21"/>
-    <mergeCell ref="AT21:AZ21"/>
-    <mergeCell ref="BB21:BC21"/>
-    <mergeCell ref="BD21:BE21"/>
-    <mergeCell ref="AF22:AJ22"/>
-    <mergeCell ref="AL22:AM22"/>
-    <mergeCell ref="AN22:AO22"/>
-    <mergeCell ref="AT22:AZ22"/>
-    <mergeCell ref="BB22:BC22"/>
-    <mergeCell ref="BD22:BE22"/>
-    <mergeCell ref="AF19:AJ19"/>
-    <mergeCell ref="AL19:AM19"/>
-    <mergeCell ref="AN19:AO19"/>
-    <mergeCell ref="AT19:AZ19"/>
-    <mergeCell ref="BB19:BC19"/>
-    <mergeCell ref="BD19:BE19"/>
-    <mergeCell ref="AF20:AJ20"/>
-    <mergeCell ref="AL20:AM20"/>
-    <mergeCell ref="AN20:AO20"/>
-    <mergeCell ref="AT20:AZ20"/>
-    <mergeCell ref="BB20:BC20"/>
-    <mergeCell ref="BD20:BE20"/>
-    <mergeCell ref="AF17:AJ17"/>
-    <mergeCell ref="AL17:AM17"/>
-    <mergeCell ref="AN17:AO17"/>
-    <mergeCell ref="AT17:AZ17"/>
-    <mergeCell ref="BB17:BC17"/>
-    <mergeCell ref="BD17:BE17"/>
-    <mergeCell ref="AF18:AJ18"/>
-    <mergeCell ref="AL18:AM18"/>
-    <mergeCell ref="AN18:AO18"/>
-    <mergeCell ref="AT18:AZ18"/>
-    <mergeCell ref="BB18:BC18"/>
-    <mergeCell ref="BD18:BE18"/>
-    <mergeCell ref="AF15:AJ15"/>
-    <mergeCell ref="AL15:AM15"/>
-    <mergeCell ref="AN15:AO15"/>
-    <mergeCell ref="AT15:AZ15"/>
-    <mergeCell ref="BB15:BC15"/>
-    <mergeCell ref="BD15:BE15"/>
-    <mergeCell ref="AF16:AJ16"/>
-    <mergeCell ref="AL16:AM16"/>
-    <mergeCell ref="AN16:AO16"/>
-    <mergeCell ref="AT16:AZ16"/>
-    <mergeCell ref="BB16:BC16"/>
-    <mergeCell ref="BD16:BE16"/>
-    <mergeCell ref="AE13:AE14"/>
-    <mergeCell ref="AF13:AJ14"/>
-    <mergeCell ref="AK13:AK14"/>
-    <mergeCell ref="AL13:AO13"/>
-    <mergeCell ref="AS13:AS14"/>
-    <mergeCell ref="AT13:AZ14"/>
-    <mergeCell ref="BA13:BA14"/>
-    <mergeCell ref="BB13:BE13"/>
-    <mergeCell ref="AL14:AM14"/>
-    <mergeCell ref="AN14:AO14"/>
-    <mergeCell ref="BB14:BC14"/>
-    <mergeCell ref="BD14:BE14"/>
     <mergeCell ref="AB8:AC8"/>
     <mergeCell ref="AD8:AD9"/>
     <mergeCell ref="A11:B11"/>
@@ -4557,6 +4448,125 @@
     <mergeCell ref="W8:W9"/>
     <mergeCell ref="X8:X9"/>
     <mergeCell ref="Y8:AA8"/>
+    <mergeCell ref="AE13:AE14"/>
+    <mergeCell ref="AF13:AJ14"/>
+    <mergeCell ref="AK13:AK14"/>
+    <mergeCell ref="AL13:AO13"/>
+    <mergeCell ref="AS13:AS14"/>
+    <mergeCell ref="AT13:AZ14"/>
+    <mergeCell ref="BA13:BA14"/>
+    <mergeCell ref="BB13:BE13"/>
+    <mergeCell ref="AL14:AM14"/>
+    <mergeCell ref="AN14:AO14"/>
+    <mergeCell ref="BB14:BC14"/>
+    <mergeCell ref="BD14:BE14"/>
+    <mergeCell ref="AF15:AJ15"/>
+    <mergeCell ref="AL15:AM15"/>
+    <mergeCell ref="AN15:AO15"/>
+    <mergeCell ref="AT15:AZ15"/>
+    <mergeCell ref="BB15:BC15"/>
+    <mergeCell ref="BD15:BE15"/>
+    <mergeCell ref="AF16:AJ16"/>
+    <mergeCell ref="AL16:AM16"/>
+    <mergeCell ref="AN16:AO16"/>
+    <mergeCell ref="AT16:AZ16"/>
+    <mergeCell ref="BB16:BC16"/>
+    <mergeCell ref="BD16:BE16"/>
+    <mergeCell ref="AF17:AJ17"/>
+    <mergeCell ref="AL17:AM17"/>
+    <mergeCell ref="AN17:AO17"/>
+    <mergeCell ref="AT17:AZ17"/>
+    <mergeCell ref="BB17:BC17"/>
+    <mergeCell ref="BD17:BE17"/>
+    <mergeCell ref="AF18:AJ18"/>
+    <mergeCell ref="AL18:AM18"/>
+    <mergeCell ref="AN18:AO18"/>
+    <mergeCell ref="AT18:AZ18"/>
+    <mergeCell ref="BB18:BC18"/>
+    <mergeCell ref="BD18:BE18"/>
+    <mergeCell ref="AF19:AJ19"/>
+    <mergeCell ref="AL19:AM19"/>
+    <mergeCell ref="AN19:AO19"/>
+    <mergeCell ref="AT19:AZ19"/>
+    <mergeCell ref="BB19:BC19"/>
+    <mergeCell ref="BD19:BE19"/>
+    <mergeCell ref="AF20:AJ20"/>
+    <mergeCell ref="AL20:AM20"/>
+    <mergeCell ref="AN20:AO20"/>
+    <mergeCell ref="AT20:AZ20"/>
+    <mergeCell ref="BB20:BC20"/>
+    <mergeCell ref="BD20:BE20"/>
+    <mergeCell ref="AF21:AJ21"/>
+    <mergeCell ref="AL21:AM21"/>
+    <mergeCell ref="AN21:AO21"/>
+    <mergeCell ref="AT21:AZ21"/>
+    <mergeCell ref="BB21:BC21"/>
+    <mergeCell ref="BD21:BE21"/>
+    <mergeCell ref="AF22:AJ22"/>
+    <mergeCell ref="AL22:AM22"/>
+    <mergeCell ref="AN22:AO22"/>
+    <mergeCell ref="AT22:AZ22"/>
+    <mergeCell ref="BB22:BC22"/>
+    <mergeCell ref="BD22:BE22"/>
+    <mergeCell ref="AF23:AJ23"/>
+    <mergeCell ref="AL23:AM23"/>
+    <mergeCell ref="AN23:AO23"/>
+    <mergeCell ref="AT23:AZ23"/>
+    <mergeCell ref="BB23:BC23"/>
+    <mergeCell ref="BD23:BE23"/>
+    <mergeCell ref="AF24:AJ24"/>
+    <mergeCell ref="AL24:AM24"/>
+    <mergeCell ref="AN24:AO24"/>
+    <mergeCell ref="AT24:AZ24"/>
+    <mergeCell ref="BB24:BC24"/>
+    <mergeCell ref="BD24:BE24"/>
+    <mergeCell ref="AF25:AJ25"/>
+    <mergeCell ref="AL25:AM25"/>
+    <mergeCell ref="AN25:AO25"/>
+    <mergeCell ref="AT25:AZ25"/>
+    <mergeCell ref="BB25:BC25"/>
+    <mergeCell ref="BD25:BE25"/>
+    <mergeCell ref="AF26:AJ26"/>
+    <mergeCell ref="AL26:AM26"/>
+    <mergeCell ref="AN26:AO26"/>
+    <mergeCell ref="AT26:AZ26"/>
+    <mergeCell ref="BB26:BC26"/>
+    <mergeCell ref="BD26:BE26"/>
+    <mergeCell ref="AF27:AJ27"/>
+    <mergeCell ref="AL27:AM27"/>
+    <mergeCell ref="AN27:AO27"/>
+    <mergeCell ref="AT27:AZ27"/>
+    <mergeCell ref="BB27:BC27"/>
+    <mergeCell ref="BD27:BE27"/>
+    <mergeCell ref="AF28:AJ28"/>
+    <mergeCell ref="AL28:AM28"/>
+    <mergeCell ref="AN28:AO28"/>
+    <mergeCell ref="AT28:AZ28"/>
+    <mergeCell ref="BB28:BC28"/>
+    <mergeCell ref="BD28:BE28"/>
+    <mergeCell ref="AF29:AJ29"/>
+    <mergeCell ref="AL29:AM29"/>
+    <mergeCell ref="AN29:AO29"/>
+    <mergeCell ref="AT29:AZ29"/>
+    <mergeCell ref="BB29:BC29"/>
+    <mergeCell ref="BD29:BE29"/>
+    <mergeCell ref="AF30:AJ30"/>
+    <mergeCell ref="AL30:AM30"/>
+    <mergeCell ref="AN30:AO30"/>
+    <mergeCell ref="AT30:AZ30"/>
+    <mergeCell ref="BB30:BC30"/>
+    <mergeCell ref="BD30:BE30"/>
+    <mergeCell ref="BD31:BE31"/>
+    <mergeCell ref="A32:AA32"/>
+    <mergeCell ref="A33:AA33"/>
+    <mergeCell ref="M34:P34"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="S34:T34"/>
+    <mergeCell ref="AF31:AJ31"/>
+    <mergeCell ref="AL31:AM31"/>
+    <mergeCell ref="AN31:AO31"/>
+    <mergeCell ref="AS31:AZ31"/>
+    <mergeCell ref="BB31:BC31"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="0" scale="24" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>